<commit_message>
thêm trường productCode + unit cho product, sửa layout
</commit_message>
<xml_diff>
--- a/public/templates/product-sample.xlsx
+++ b/public/templates/product-sample.xlsx
@@ -16,17 +16,62 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Mô tả sản phẩm 1</t>
-  </si>
-  <si>
-    <t>Mô tả sản phẩm 2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+  <si>
+    <t>Sản phẩm A</t>
+  </si>
+  <si>
+    <t>Mô tả sản phẩm A</t>
+  </si>
+  <si>
+    <t>Danh mục A</t>
+  </si>
+  <si>
+    <t>cái</t>
+  </si>
+  <si>
+    <t>Sản phẩm B</t>
+  </si>
+  <si>
+    <t>Mô tả sản phẩm B</t>
+  </si>
+  <si>
+    <t>Danh mục B</t>
+  </si>
+  <si>
+    <t>hộp</t>
+  </si>
+  <si>
+    <t>Sản phẩm C</t>
+  </si>
+  <si>
+    <t>Mô tả sản phẩm C</t>
+  </si>
+  <si>
+    <t>Danh mục C</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Sản phẩm D</t>
+  </si>
+  <si>
+    <t>Mô tả sản phẩm D</t>
+  </si>
+  <si>
+    <t>Chưa phân loại</t>
+  </si>
+  <si>
+    <t>gói</t>
   </si>
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>productCode</t>
+  </si>
+  <si>
     <t>description</t>
   </si>
   <si>
@@ -39,16 +84,22 @@
     <t>category</t>
   </si>
   <si>
+    <t>unit</t>
+  </si>
+  <si>
     <t>discountPercentage</t>
   </si>
   <si>
-    <t>Động vật</t>
-  </si>
-  <si>
-    <t>Sản phẩm mẫu 1</t>
-  </si>
-  <si>
-    <t>Sản phẩm mẫu 2</t>
+    <t>SAN-2908</t>
+  </si>
+  <si>
+    <t>SAN-9564</t>
+  </si>
+  <si>
+    <t>SAN-5425</t>
+  </si>
+  <si>
+    <t>SAN-2712</t>
   </si>
 </sst>
 </file>
@@ -92,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -101,7 +152,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,63 +478,145 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
-        <v>10000</v>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D2" s="3">
+        <v>100000</v>
+      </c>
+      <c r="E2" s="3">
         <v>50</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3">
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>200000</v>
+      </c>
+      <c r="E3" s="3">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3">
+        <v>150000</v>
+      </c>
+      <c r="E4" s="3">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>20000</v>
-      </c>
-      <c r="D3" s="3">
-        <v>30</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3">
-        <v>5</v>
-      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3">
+        <v>50000</v>
+      </c>
+      <c r="E5" s="3">
+        <v>100</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>